<commit_message>
create posts, edit data structure
</commit_message>
<xml_diff>
--- a/documents/DataStructure.xlsx
+++ b/documents/DataStructure.xlsx
@@ -29,9 +29,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>FanPageSNP</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -132,19 +129,28 @@
   </si>
   <si>
     <t>[Like]</t>
+  </si>
+  <si>
+    <t>snp_fanpage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -261,68 +267,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,420 +630,421 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2" t="s">
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
+      <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="17" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="17" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
-      <c r="B27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A37:A44"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A18"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="A28:A36"/>
-    <mergeCell ref="A37:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>